<commit_message>
save keys and retrieve back
</commit_message>
<xml_diff>
--- a/pw.xlsx
+++ b/pw.xlsx
@@ -939,11 +939,11 @@
   </sheetPr>
   <dimension ref="A1:I1160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.11"/>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">MAX(G2:G162)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>